<commit_message>
sops 2 and 3
</commit_message>
<xml_diff>
--- a/1-Software Development Lifecycle/Forms/Request Meeting In Mintues Form F2.xlsx
+++ b/1-Software Development Lifecycle/Forms/Request Meeting In Mintues Form F2.xlsx
@@ -5,18 +5,18 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heba.backar\Downloads\SW 2025 2\SW 2025\SW 2025\1-Software Development Lifecycle\Forms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heba.backar\Desktop\QMS Forms Github\SOPs\1-Software Development Lifecycle\Forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{663086A6-64A2-4B49-8FDE-08059A79ACD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B11125-3285-4A6E-9D2A-DB4625747CD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{002BD202-C88A-4287-BFF3-25B76F21E7BF}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{002BD202-C88A-4287-BFF3-25B76F21E7BF}"/>
   </bookViews>
   <sheets>
     <sheet name="F-SW-SD-02" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'F-SW-SD-02'!$A$1:$I$32</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'F-SW-SD-02'!$A$1:$I$33</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Agenda:</t>
   </si>
@@ -88,12 +88,15 @@
   <si>
     <t>Request ID:</t>
   </si>
+  <si>
+    <t>Request Type:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,6 +136,19 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -250,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -262,19 +278,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -289,27 +296,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -319,11 +305,47 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -737,10 +759,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE062CB-69B9-4769-9071-7E7FB1DB25B4}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L591"/>
+  <dimension ref="A1:L592"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" topLeftCell="A2" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:I10"/>
+      <selection activeCell="C5" sqref="C5:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,475 +779,473 @@
   <sheetData>
     <row r="1" spans="1:12" ht="70.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-    </row>
-    <row r="4" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="B3" s="16"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+    </row>
+    <row r="4" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="28"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+    </row>
+    <row r="5" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-    </row>
-    <row r="5" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="19"/>
+      <c r="B5" s="1"/>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
-      <c r="E5" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="19" t="s">
-        <v>6</v>
+    <row r="6" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="16" t="s">
+        <v>4</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19" t="s">
-        <v>9</v>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="23" t="s">
+        <v>5</v>
       </c>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="19" t="s">
-        <v>7</v>
+    <row r="7" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="16" t="s">
+        <v>6</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
+    <row r="8" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-    </row>
-    <row r="9" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
+      <c r="B9" s="20"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+    </row>
+    <row r="10" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-    </row>
-    <row r="10" spans="1:12" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="26"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="25"/>
+    <row r="11" spans="1:12" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="11"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="12"/>
+    <row r="12" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="15"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="11"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="12"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="9"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="11"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="12"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="9"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="11"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="12"/>
+    <row r="15" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="9"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="1:12" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A16" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="25"/>
+    <row r="16" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="9"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
     </row>
-    <row r="17" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A17" s="11"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="12"/>
+    <row r="17" spans="1:12" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A17" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="15"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
     </row>
     <row r="18" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="11"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="12"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="9"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
     </row>
     <row r="19" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="11"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="12"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="9"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
     </row>
-    <row r="20" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="13"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="15"/>
+    <row r="20" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A20" s="7"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="9"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
     </row>
-    <row r="21" spans="1:12" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="4"/>
+    <row r="21" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="10"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="12"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="11"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="12"/>
+    <row r="22" spans="1:12" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="4"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
     </row>
     <row r="23" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="11"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="12"/>
+      <c r="A23" s="7"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="9"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
     </row>
     <row r="24" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A24" s="11"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="12"/>
+      <c r="A24" s="7"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="9"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
     </row>
-    <row r="25" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="13"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="15"/>
+    <row r="25" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A25" s="7"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="9"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
     </row>
-    <row r="26" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="25"/>
+    <row r="26" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="10"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="12"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
     </row>
     <row r="27" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="16"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="16"/>
+      <c r="A27" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="15"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
     </row>
     <row r="28" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="16"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
+      <c r="A28" s="26"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="26"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
     </row>
     <row r="29" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="16"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
+      <c r="A29" s="26"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
     </row>
-    <row r="30" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="17"/>
+    <row r="30" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="26"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
     </row>
     <row r="31" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="9" t="s">
-        <v>4</v>
+      <c r="A31" s="6" t="s">
+        <v>12</v>
       </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
     </row>
     <row r="32" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A32" s="7" t="s">
-        <v>13</v>
+      <c r="A32" s="17" t="s">
+        <v>4</v>
       </c>
-      <c r="B32" s="7"/>
+      <c r="B32" s="17"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
       <c r="H32" s="8"/>
-      <c r="I32" s="5"/>
+      <c r="I32" s="8"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
     </row>
     <row r="33" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
+      <c r="A33" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="24"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="25"/>
+      <c r="H33" s="25"/>
+      <c r="I33" s="5"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
@@ -9042,33 +9062,49 @@
       <c r="K591" s="1"/>
       <c r="L591" s="1"/>
     </row>
+    <row r="592" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A592" s="1"/>
+      <c r="B592" s="1"/>
+      <c r="C592" s="1"/>
+      <c r="D592" s="1"/>
+      <c r="E592" s="1"/>
+      <c r="F592" s="1"/>
+      <c r="G592" s="1"/>
+      <c r="H592" s="1"/>
+      <c r="I592" s="1"/>
+      <c r="J592" s="1"/>
+      <c r="K592" s="1"/>
+      <c r="L592" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="A17:I20"/>
-    <mergeCell ref="A26:I26"/>
+  <mergeCells count="27">
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:H33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:I32"/>
+    <mergeCell ref="A23:I26"/>
+    <mergeCell ref="A28:I30"/>
+    <mergeCell ref="C31:I31"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A6:D6"/>
     <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A16:I16"/>
-    <mergeCell ref="A11:I11"/>
-    <mergeCell ref="A9:I10"/>
-    <mergeCell ref="A12:I15"/>
-    <mergeCell ref="E7:I7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:H8"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A6:D6"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:H3"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="E6:I6"/>
+    <mergeCell ref="E7:I7"/>
+    <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:H4"/>
-    <mergeCell ref="E5:I5"/>
-    <mergeCell ref="E6:I6"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:H32"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:I31"/>
-    <mergeCell ref="A22:I25"/>
-    <mergeCell ref="A27:I29"/>
-    <mergeCell ref="C30:I30"/>
+    <mergeCell ref="A18:I21"/>
+    <mergeCell ref="A27:I27"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A17:I17"/>
+    <mergeCell ref="A12:I12"/>
+    <mergeCell ref="A10:I11"/>
+    <mergeCell ref="A13:I16"/>
+    <mergeCell ref="E8:I8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:H9"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.5" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>